<commit_message>
Castes into/from CMS. (#59)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A05410-B638-4D48-8DDF-55EB84CB04FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7271F627-AF9F-4651-9E66-AFEBFE324AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Abruti, Adresse légendaire</t>
+  </si>
+  <si>
+    <t>Amuseur</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,9 @@
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>

</xml_diff>

<commit_message>
Educations into/from CMS. (#60)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7271F627-AF9F-4651-9E66-AFEBFE324AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F9FF1E-A3B8-40C7-8935-95641BED4ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="34560" windowHeight="18600" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Progression" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -81,13 +81,16 @@
   </si>
   <si>
     <t>Amuseur</t>
+  </si>
+  <si>
+    <t>Apprenti à l’étranger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +113,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +137,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -154,11 +169,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,9 +191,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -591,7 +611,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>

</xml_diff>

<commit_message>
Refactored Skills & Lineages. (#64)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BC0BB1-694B-4E8F-9F65-BB3642C1B31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D87FDF0-908E-47D5-A538-74301751ADF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Apprentissage</t>
+  </si>
+  <si>
+    <t>Acrobaties</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,9 @@
         <v>45932</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="6" t="s">

</xml_diff>

<commit_message>
October 2nd Work. (#67)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D87FDF0-908E-47D5-A538-74301751ADF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D34F5B-CE6A-4360-93DE-1A3CC3C688D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>Acrobaties</t>
+  </si>
+  <si>
+    <t>Charlatan</t>
+  </si>
+  <si>
+    <t>Affinité animale</t>
+  </si>
+  <si>
+    <t>Costaud</t>
+  </si>
+  <si>
+    <t>Armes à deux mains</t>
+  </si>
+  <si>
+    <t>Éclaireur</t>
   </si>
 </sst>
 </file>
@@ -662,24 +677,34 @@
       <c r="A3" s="4">
         <v>45932</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4">

</xml_diff>

<commit_message>
October 3rd Work. (#68)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D34F5B-CE6A-4360-93DE-1A3CC3C688D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D827E0F8-2C4F-47DA-9F13-33514BF41C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,30 @@
   </si>
   <si>
     <t>Éclaireur</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Artisanat</t>
+  </si>
+  <si>
+    <t>Cuirassé</t>
+  </si>
+  <si>
+    <t>Élémentariste</t>
+  </si>
+  <si>
+    <t>Armes de finesse</t>
+  </si>
+  <si>
+    <t>Apprenti d’un maître</t>
+  </si>
+  <si>
+    <t>Aigrefin</t>
   </si>
 </sst>
 </file>
@@ -710,18 +734,34 @@
       <c r="A4" s="4">
         <v>45933</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4">

</xml_diff>

<commit_message>
October 4th Work. (#69)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D827E0F8-2C4F-47DA-9F13-33514BF41C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1683D5D-4290-4310-94D5-EB6F6DFDF456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,30 @@
   </si>
   <si>
     <t>Aigrefin</t>
+  </si>
+  <si>
+    <t>Enterainer</t>
+  </si>
+  <si>
+    <t>Énergie</t>
+  </si>
+  <si>
+    <t>Anxiété, Aveugle</t>
+  </si>
+  <si>
+    <t>Champs de bataille</t>
+  </si>
+  <si>
+    <t>Arts martiaux</t>
+  </si>
+  <si>
+    <t>Culbutes</t>
+  </si>
+  <si>
+    <t>Armes de jet</t>
+  </si>
+  <si>
+    <t>Ménestrel</t>
   </si>
 </sst>
 </file>
@@ -767,18 +791,34 @@
       <c r="A5" s="4">
         <v>45934</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4">

</xml_diff>

<commit_message>
October 5th Work. (#70)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1683D5D-4290-4310-94D5-EB6F6DFDF456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF40F1C3-38AD-4A1A-B2D9-021F28E8D6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -171,6 +171,30 @@
   </si>
   <si>
     <t>Ménestrel</t>
+  </si>
+  <si>
+    <t>Roublard</t>
+  </si>
+  <si>
+    <t>Folk Hero</t>
+  </si>
+  <si>
+    <t>Esquive</t>
+  </si>
+  <si>
+    <t>Baraqué</t>
+  </si>
+  <si>
+    <t>Classique</t>
+  </si>
+  <si>
+    <t>Athlétisme</t>
+  </si>
+  <si>
+    <t>Attaque sournoise</t>
+  </si>
+  <si>
+    <t>Distraction</t>
   </si>
 </sst>
 </file>
@@ -824,18 +848,34 @@
       <c r="A6" s="4">
         <v>45935</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="B6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4">

</xml_diff>

<commit_message>
October 6th Work. (#71)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF40F1C3-38AD-4A1A-B2D9-021F28E8D6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CA1202-CB0B-420E-B426-7BBC6DC5B33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,30 @@
   </si>
   <si>
     <t>Distraction</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>Guild Artisan</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Dans la rue</t>
+  </si>
+  <si>
+    <t>Bricolage magique</t>
+  </si>
+  <si>
+    <t>Emboîter le pas</t>
+  </si>
+  <si>
+    <t>Attaque neutralisante</t>
+  </si>
+  <si>
+    <t>Borgne, Chance extraordinaire</t>
   </si>
 </sst>
 </file>
@@ -881,18 +905,34 @@
       <c r="A7" s="4">
         <v>45936</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="B7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4">

</xml_diff>

<commit_message>
October 7th Work. (#72)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CA1202-CB0B-420E-B426-7BBC6DC5B33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44596D40-5BBB-4C92-A43C-2669D77B0FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,30 @@
   </si>
   <si>
     <t>Borgne, Chance extraordinaire</t>
+  </si>
+  <si>
+    <t>Augure</t>
+  </si>
+  <si>
+    <t>Hermit</t>
+  </si>
+  <si>
+    <t>Initiative</t>
+  </si>
+  <si>
+    <t>Combinaison élémentaire</t>
+  </si>
+  <si>
+    <t>Endurance accrue</t>
+  </si>
+  <si>
+    <t>Entreprise familiale</t>
+  </si>
+  <si>
+    <t>Chaotique</t>
+  </si>
+  <si>
+    <t>Attaque puissante</t>
   </si>
 </sst>
 </file>
@@ -938,18 +962,34 @@
       <c r="A8" s="4">
         <v>45937</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="B8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4">

</xml_diff>

<commit_message>
October 8th Work. (#73)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44596D40-5BBB-4C92-A43C-2669D77B0FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA3D6FF-4904-4EA0-90E9-E25FED08D939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,32 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Personnalisation (3,26)</t>
-  </si>
-  <si>
     <t>SEO Stats / Skills (1)</t>
   </si>
   <si>
-    <t>SEO Talents T0 (1.23)</t>
-  </si>
-  <si>
-    <t>SEO Talents T1 (0.9)</t>
-  </si>
-  <si>
-    <t>Talents T1 (0.74)</t>
-  </si>
-  <si>
     <t>Castes / Éduc. (0.65)</t>
   </si>
   <si>
-    <t>Dons &amp; Handic. (1.48)</t>
-  </si>
-  <si>
     <t>Astromancie (3.23%)</t>
   </si>
   <si>
@@ -92,9 +77,6 @@
     <t>Armes de tir</t>
   </si>
   <si>
-    <t>Ambidextre</t>
-  </si>
-  <si>
     <t>Astrologie</t>
   </si>
   <si>
@@ -119,9 +101,6 @@
     <t>Costaud</t>
   </si>
   <si>
-    <t>Armes à deux mains</t>
-  </si>
-  <si>
     <t>Éclaireur</t>
   </si>
   <si>
@@ -167,9 +146,6 @@
     <t>Culbutes</t>
   </si>
   <si>
-    <t>Armes de jet</t>
-  </si>
-  <si>
     <t>Ménestrel</t>
   </si>
   <si>
@@ -191,9 +167,6 @@
     <t>Athlétisme</t>
   </si>
   <si>
-    <t>Attaque sournoise</t>
-  </si>
-  <si>
     <t>Distraction</t>
   </si>
   <si>
@@ -242,14 +215,68 @@
     <t>Chaotique</t>
   </si>
   <si>
-    <t>Attaque puissante</t>
+    <t>Noble</t>
+  </si>
+  <si>
+    <t>Précision</t>
+  </si>
+  <si>
+    <t>Judicieux</t>
+  </si>
+  <si>
+    <t>Compétence, Connaissance</t>
+  </si>
+  <si>
+    <t>Enquête</t>
+  </si>
+  <si>
+    <t>Personnalisation</t>
+  </si>
+  <si>
+    <t>Dons &amp; Handic. (1.5)</t>
+  </si>
+  <si>
+    <t>SEO Talents T0 (1.25)</t>
+  </si>
+  <si>
+    <t>SEO Talents T1 (1)</t>
+  </si>
+  <si>
+    <t>Talents T1 (1.5)</t>
+  </si>
+  <si>
+    <t>Bricoleur</t>
+  </si>
+  <si>
+    <t>Ambidextre, Armes à deux mains</t>
+  </si>
+  <si>
+    <t>Armes de jet, Attaque sournoise</t>
+  </si>
+  <si>
+    <t>Attaque puissante, Barrière mentale</t>
+  </si>
+  <si>
+    <t>Bris</t>
+  </si>
+  <si>
+    <t>Charge, Coup de bouclier</t>
+  </si>
+  <si>
+    <t>Critique accru</t>
+  </si>
+  <si>
+    <t>Frappe puissante</t>
+  </si>
+  <si>
+    <t>Chétif, Santé de fer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +309,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -346,7 +381,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,6 +402,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -716,7 +754,9 @@
     <col min="5" max="5" width="25.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" style="1"/>
     <col min="7" max="7" width="25.77734375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="19.5546875" style="1"/>
+    <col min="8" max="8" width="19.5546875" style="1"/>
+    <col min="9" max="9" width="32" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="19.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -724,40 +764,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -765,29 +805,29 @@
         <v>45931</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -798,29 +838,29 @@
         <v>45932</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
@@ -831,29 +871,29 @@
         <v>45933</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -864,29 +904,29 @@
         <v>45934</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -897,29 +937,29 @@
         <v>45935</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -930,29 +970,29 @@
         <v>45936</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>53</v>
+        <v>76</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -963,29 +1003,29 @@
         <v>45937</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -995,18 +1035,34 @@
       <c r="A9" s="4">
         <v>45938</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="B9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -1393,7 +1449,9 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>

</xml_diff>

<commit_message>
October 9th Work. (#81)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA3D6FF-4904-4EA0-90E9-E25FED08D939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AB372C-9349-4C77-9BC8-1C9D8BCBE578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -270,6 +270,30 @@
   </si>
   <si>
     <t>Chétif, Santé de fer</t>
+  </si>
+  <si>
+    <t>Outlander</t>
+  </si>
+  <si>
+    <t>Puissance</t>
+  </si>
+  <si>
+    <t>Coup critique</t>
+  </si>
+  <si>
+    <t>Brigand</t>
+  </si>
+  <si>
+    <t>Entraînement II</t>
+  </si>
+  <si>
+    <t>Infusions magiques</t>
+  </si>
+  <si>
+    <t>Cleptomane</t>
+  </si>
+  <si>
+    <t>Mentor vénérable</t>
   </si>
 </sst>
 </file>
@@ -1068,18 +1092,34 @@
       <c r="A10" s="4">
         <v>45939</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="B10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -1090,7 +1130,9 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>

</xml_diff>

<commit_message>
October 10th Work. (#82)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AB372C-9349-4C77-9BC8-1C9D8BCBE578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74ADDAE-CC33-4D83-8F5B-1F6733211D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -294,6 +294,33 @@
   </si>
   <si>
     <t>Mentor vénérable</t>
+  </si>
+  <si>
+    <t>Entraînement I</t>
+  </si>
+  <si>
+    <t>Sage</t>
+  </si>
+  <si>
+    <t>Stratagème</t>
+  </si>
+  <si>
+    <t>Distrait</t>
+  </si>
+  <si>
+    <t>Rebelle</t>
+  </si>
+  <si>
+    <t>Expertise artisanale</t>
+  </si>
+  <si>
+    <t>Initiation magique</t>
+  </si>
+  <si>
+    <t>Attaque brutale, Lancer brutal</t>
+  </si>
+  <si>
+    <t>Brute</t>
   </si>
 </sst>
 </file>
@@ -1125,20 +1152,34 @@
       <c r="A11" s="4">
         <v>45940</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="B11" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="G11" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -1474,7 +1515,9 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>

</xml_diff>

<commit_message>
October 11th Work. (#83)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74ADDAE-CC33-4D83-8F5B-1F6733211D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE52766-42E8-4EBD-98FA-896F5C4FDB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
   <si>
     <t>Date</t>
   </si>
@@ -321,6 +321,105 @@
   </si>
   <si>
     <t>Brute</t>
+  </si>
+  <si>
+    <t>Sous contrainte</t>
+  </si>
+  <si>
+    <t>Sailor</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>Urchin</t>
+  </si>
+  <si>
+    <t>Other Backgrounds</t>
+  </si>
+  <si>
+    <t>Vitalité</t>
+  </si>
+  <si>
+    <t>Entrepôt à connaissances</t>
+  </si>
+  <si>
+    <t>Dur à cuire, Effacé</t>
+  </si>
+  <si>
+    <t>Faiblesse, Féroce</t>
+  </si>
+  <si>
+    <t>Fignolage, Globe-trotteur</t>
+  </si>
+  <si>
+    <t>Artisan</t>
+  </si>
+  <si>
+    <t>Bohème</t>
+  </si>
+  <si>
+    <t>Exilé</t>
+  </si>
+  <si>
+    <t>Guérisseur</t>
+  </si>
+  <si>
+    <t>Marchand</t>
+  </si>
+  <si>
+    <t>Milicien</t>
+  </si>
+  <si>
+    <t>Paysan</t>
+  </si>
+  <si>
+    <t>Religieux</t>
+  </si>
+  <si>
+    <t>Connaissance</t>
+  </si>
+  <si>
+    <t>Diplomatie</t>
+  </si>
+  <si>
+    <t>Discipline</t>
+  </si>
+  <si>
+    <t>Furtivité</t>
+  </si>
+  <si>
+    <t>Intuition</t>
+  </si>
+  <si>
+    <t>Investigation</t>
+  </si>
+  <si>
+    <t>Linguistique</t>
+  </si>
+  <si>
+    <t>Dressage</t>
+  </si>
+  <si>
+    <t>Élémentarisme</t>
+  </si>
+  <si>
+    <t>Herboristerie</t>
+  </si>
+  <si>
+    <t>Initiative accrue</t>
+  </si>
+  <si>
+    <t>Lutte</t>
+  </si>
+  <si>
+    <t>Cambrioleur</t>
+  </si>
+  <si>
+    <t>Catalyste</t>
+  </si>
+  <si>
+    <t>Chaman</t>
   </si>
 </sst>
 </file>
@@ -1185,171 +1284,253 @@
       <c r="A12" s="4">
         <v>45941</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="B12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>45942</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="B13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45943</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="B14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>45944</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>45945</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45946</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="B17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45947</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="B18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>45948</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>45949</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>45950</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4">

</xml_diff>

<commit_message>
October 12th Work. (#84)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE52766-42E8-4EBD-98FA-896F5C4FDB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1F494-536E-4AC9-AB3B-12EB05739722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="168">
   <si>
     <t>Date</t>
   </si>
@@ -398,9 +398,6 @@
     <t>Linguistique</t>
   </si>
   <si>
-    <t>Dressage</t>
-  </si>
-  <si>
     <t>Élémentarisme</t>
   </si>
   <si>
@@ -420,6 +417,129 @@
   </si>
   <si>
     <t>Chaman</t>
+  </si>
+  <si>
+    <t>Médecine animale, Méditation</t>
+  </si>
+  <si>
+    <t>Magie puissante</t>
+  </si>
+  <si>
+    <t>Maraudage</t>
+  </si>
+  <si>
+    <t>Parade</t>
+  </si>
+  <si>
+    <t>Paréidolie</t>
+  </si>
+  <si>
+    <t>Méta-magie</t>
+  </si>
+  <si>
+    <t>Méfait feutré</t>
+  </si>
+  <si>
+    <t>Naturalisme</t>
+  </si>
+  <si>
+    <t>Observateur</t>
+  </si>
+  <si>
+    <t>Philologie</t>
+  </si>
+  <si>
+    <t>Présence terrifiante</t>
+  </si>
+  <si>
+    <t>Renvoi des m.-v.</t>
+  </si>
+  <si>
+    <t>Robustesse accrue</t>
+  </si>
+  <si>
+    <t>Société</t>
+  </si>
+  <si>
+    <t>Survivalisme</t>
+  </si>
+  <si>
+    <t>Suspicion</t>
+  </si>
+  <si>
+    <t>Tir rapide</t>
+  </si>
+  <si>
+    <t>Tissu de mensonges</t>
+  </si>
+  <si>
+    <t>Tolérance à l'alcool II</t>
+  </si>
+  <si>
+    <t>Discipline, Dressage</t>
+  </si>
+  <si>
+    <t>Formation martiale</t>
+  </si>
+  <si>
+    <t>Expertise, Furtivité</t>
+  </si>
+  <si>
+    <t>Illusions mineures</t>
+  </si>
+  <si>
+    <t>Intuition, Investigation</t>
+  </si>
+  <si>
+    <t>Langue supplémentaire</t>
+  </si>
+  <si>
+    <t>Médecine</t>
+  </si>
+  <si>
+    <t>Mêlée, Orientation</t>
+  </si>
+  <si>
+    <t>Occultisme</t>
+  </si>
+  <si>
+    <t>Perception</t>
+  </si>
+  <si>
+    <t>Représentation</t>
+  </si>
+  <si>
+    <t>Résistance, Survie</t>
+  </si>
+  <si>
+    <t>Roublardise</t>
+  </si>
+  <si>
+    <t>Spiritualité</t>
+  </si>
+  <si>
+    <t>Tolérance à l'alcool I</t>
+  </si>
+  <si>
+    <t>Tromperie</t>
+  </si>
+  <si>
+    <t>Trousses</t>
+  </si>
+  <si>
+    <t>Vigilance</t>
+  </si>
+  <si>
+    <t>Mêlée</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>Résistance</t>
+  </si>
+  <si>
+    <t>Survie</t>
   </si>
 </sst>
 </file>
@@ -531,15 +651,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -951,777 +1068,889 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>45931</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>45932</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>45933</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>45934</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>45935</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>45936</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>45937</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>45938</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>45939</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>45940</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>45941</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>45942</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="J12" s="6" t="s">
+      <c r="I13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>45942</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>45943</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>45944</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>45945</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>45946</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>45943</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>45944</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>45947</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>45945</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>45946</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>45947</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="G18" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>45948</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="G19" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>45949</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="G20" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>45950</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="G21" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>45951</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>45952</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>45953</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>45954</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>45955</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>45956</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>45957</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>45958</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>45959</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>45960</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="6" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>45961</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="6" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
October 13th Work. (#85)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1F494-536E-4AC9-AB3B-12EB05739722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E5B1FB-3FCB-4A30-828D-8769B06DA445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
   <si>
     <t>Date</t>
   </si>
@@ -540,6 +540,12 @@
   </si>
   <si>
     <t>Survie</t>
+  </si>
+  <si>
+    <t>Chasseur</t>
+  </si>
+  <si>
+    <t>Druide</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84369EDC-CDC8-4C47-A733-5DEB44CD56DA}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1470,14 +1478,14 @@
       <c r="B14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1486,7 +1494,9 @@
       <c r="H14" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="J14" s="5" t="s">
         <v>126</v>
       </c>
@@ -1518,7 +1528,9 @@
         <v>129</v>
       </c>
       <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>168</v>
+      </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -1545,7 +1557,9 @@
         <v>133</v>
       </c>
       <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -1848,9 +1862,7 @@
       <c r="H28" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>131</v>
-      </c>
+      <c r="I28" s="5"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -1874,7 +1886,7 @@
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>

</xml_diff>

<commit_message>
October 14th Work. (#86)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E5B1FB-3FCB-4A30-828D-8769B06DA445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3072A428-76DA-40BE-B7C4-E825B2656DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -257,9 +257,6 @@
     <t>Attaque puissante, Barrière mentale</t>
   </si>
   <si>
-    <t>Bris</t>
-  </si>
-  <si>
     <t>Charge, Coup de bouclier</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>Expertise artisanale</t>
   </si>
   <si>
-    <t>Initiation magique</t>
-  </si>
-  <si>
     <t>Attaque brutale, Lancer brutal</t>
   </si>
   <si>
@@ -431,12 +425,6 @@
     <t>Parade</t>
   </si>
   <si>
-    <t>Paréidolie</t>
-  </si>
-  <si>
-    <t>Méta-magie</t>
-  </si>
-  <si>
     <t>Méfait feutré</t>
   </si>
   <si>
@@ -546,13 +534,25 @@
   </si>
   <si>
     <t>Druide</t>
+  </si>
+  <si>
+    <t>Champion</t>
+  </si>
+  <si>
+    <t>Bris, Paréidolie</t>
+  </si>
+  <si>
+    <t>Initiation magique, Méta-magie</t>
+  </si>
+  <si>
+    <t>Talents T2 (2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,6 +593,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,7 +665,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,6 +686,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1017,11 +1028,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84369EDC-CDC8-4C47-A733-5DEB44CD56DA}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1264,7 +1273,7 @@
         <v>49</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>44</v>
@@ -1297,7 +1306,7 @@
         <v>56</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>52</v>
@@ -1318,7 +1327,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>61</v>
@@ -1330,7 +1339,7 @@
         <v>63</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>69</v>
@@ -1344,29 +1353,29 @@
         <v>45939</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="G10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1377,29 +1386,29 @@
         <v>45940</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1410,29 +1419,29 @@
         <v>45941</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="J12" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1443,29 +1452,29 @@
         <v>45942</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="G13" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1476,29 +1485,29 @@
         <v>45943</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1509,27 +1518,29 @@
         <v>45944</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>113</v>
+        <v>97</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>107</v>
+      <c r="E15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6" t="s">
-        <v>168</v>
+        <v>127</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1540,25 +1551,27 @@
         <v>45945</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="7" t="s">
-        <v>169</v>
+        <v>129</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -1569,24 +1582,26 @@
         <v>45946</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
+      <c r="J17" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -1596,21 +1611,21 @@
         <v>45947</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
@@ -1624,7 +1639,7 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1632,10 +1647,10 @@
         <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
@@ -1649,18 +1664,18 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="6"/>
@@ -1674,18 +1689,18 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1699,7 +1714,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1707,10 +1722,10 @@
         <v>10</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1724,7 +1739,7 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1732,10 +1747,10 @@
         <v>28</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -1749,7 +1764,7 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1757,10 +1772,10 @@
         <v>33</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="6"/>
@@ -1774,7 +1789,7 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1782,10 +1797,10 @@
         <v>41</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="6"/>
@@ -1799,7 +1814,7 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1807,10 +1822,10 @@
         <v>47</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="6"/>
@@ -1824,7 +1839,7 @@
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1832,10 +1847,10 @@
         <v>57</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="6"/>
@@ -1849,7 +1864,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1857,10 +1872,10 @@
         <v>61</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="6"/>
@@ -1874,20 +1889,18 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="5" t="s">
-        <v>131</v>
-      </c>
+      <c r="I29" s="5"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
@@ -1899,20 +1912,18 @@
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H30" s="5"/>
-      <c r="I30" s="5" t="s">
-        <v>132</v>
-      </c>
+      <c r="I30" s="5"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
@@ -1924,20 +1935,18 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="I31" s="5"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
@@ -1953,16 +1962,19 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="I32" s="5"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="8" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
October 15th Work. (#87)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3072A428-76DA-40BE-B7C4-E825B2656DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7283C2D1-F1C8-4577-9C38-D6FC8021F430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="186">
   <si>
     <t>Date</t>
   </si>
@@ -546,6 +546,54 @@
   </si>
   <si>
     <t>Talents T2 (2)</t>
+  </si>
+  <si>
+    <t>Infatigable, Infirme</t>
+  </si>
+  <si>
+    <t>Alchimie, Artillerie</t>
+  </si>
+  <si>
+    <t>Attaque incapacitante / sanglante</t>
+  </si>
+  <si>
+    <t>Attaque magie / précise</t>
+  </si>
+  <si>
+    <t>Frappe précise, Lancer précis</t>
+  </si>
+  <si>
+    <t>Critique supérieur, Initiative supérieure</t>
+  </si>
+  <si>
+    <t>Attaques multiples, Double attaque</t>
+  </si>
+  <si>
+    <t>Magie guerrière, Magie précise</t>
+  </si>
+  <si>
+    <t>Monture de combat, Obé. ànimale</t>
+  </si>
+  <si>
+    <t>Érudition, Mythologie</t>
+  </si>
+  <si>
+    <t>Onde de choc, Otage</t>
+  </si>
+  <si>
+    <t>Apothicairerie, Toxicologie</t>
+  </si>
+  <si>
+    <t>Chasse-mage, Sentinelle</t>
+  </si>
+  <si>
+    <t>Blindé, Protection</t>
+  </si>
+  <si>
+    <t>Interrogateur, Résilience</t>
+  </si>
+  <si>
+    <t>Accélération, Chargement rapide</t>
   </si>
 </sst>
 </file>
@@ -635,7 +683,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -654,6 +702,90 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -665,7 +797,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -685,10 +817,43 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1043,7 +1208,7 @@
     <col min="10" max="16384" width="19.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1233,7 @@
       <c r="H1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>68</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1104,13 +1269,13 @@
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="6"/>
@@ -1137,13 +1302,13 @@
       <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="6"/>
@@ -1170,13 +1335,13 @@
       <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="6"/>
@@ -1203,13 +1368,13 @@
       <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="K5" s="6"/>
@@ -1236,13 +1401,13 @@
       <c r="G6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="9" t="s">
         <v>37</v>
       </c>
       <c r="K6" s="6"/>
@@ -1269,13 +1434,13 @@
       <c r="G7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="K7" s="6"/>
@@ -1302,13 +1467,13 @@
       <c r="G8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="10" t="s">
         <v>52</v>
       </c>
       <c r="K8" s="6"/>
@@ -1335,13 +1500,13 @@
       <c r="G9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="11" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="6"/>
@@ -1368,13 +1533,13 @@
       <c r="G10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="11" t="s">
         <v>80</v>
       </c>
       <c r="K10" s="6"/>
@@ -1401,13 +1566,13 @@
       <c r="G11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="11" t="s">
         <v>92</v>
       </c>
       <c r="K11" s="6"/>
@@ -1434,13 +1599,13 @@
       <c r="G12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="11" t="s">
         <v>122</v>
       </c>
       <c r="K12" s="6"/>
@@ -1467,13 +1632,13 @@
       <c r="G13" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="11" t="s">
         <v>123</v>
       </c>
       <c r="K13" s="6"/>
@@ -1500,13 +1665,13 @@
       <c r="G14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="11" t="s">
         <v>124</v>
       </c>
       <c r="K14" s="6"/>
@@ -1533,44 +1698,46 @@
       <c r="G15" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="11" t="s">
         <v>166</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>45945</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="11" t="s">
         <v>164</v>
       </c>
       <c r="K16" s="6"/>
@@ -1588,18 +1755,22 @@
         <v>113</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
       <c r="F17" s="6" t="s">
         <v>107</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="7" t="s">
+      <c r="I17" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="10" t="s">
         <v>165</v>
       </c>
       <c r="K17" s="6"/>
@@ -1617,18 +1788,22 @@
         <v>114</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>2</v>
+      </c>
       <c r="F18" s="6" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
+      <c r="I18" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="J18" s="17"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -1642,18 +1817,22 @@
         <v>115</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
       <c r="F19" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="I19" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="17"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1667,18 +1846,22 @@
         <v>116</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>2</v>
+      </c>
       <c r="F20" s="6" t="s">
         <v>109</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
+      <c r="I20" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" s="17"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -1692,18 +1875,22 @@
         <v>117</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
       <c r="F21" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
+      <c r="I21" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="J21" s="17"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -1717,18 +1904,22 @@
         <v>148</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>2</v>
+      </c>
       <c r="F22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6"/>
+      <c r="I22" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J22" s="17"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -1742,18 +1933,22 @@
         <v>160</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
       <c r="F23" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="6"/>
+      <c r="I23" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="J23" s="17"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -1767,18 +1962,22 @@
         <v>150</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6">
+        <v>2</v>
+      </c>
       <c r="F24" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="6"/>
+      <c r="I24" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="J24" s="17"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1792,18 +1991,22 @@
         <v>161</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
       <c r="F25" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6"/>
+      <c r="I25" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="J25" s="17"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -1817,18 +2020,22 @@
         <v>151</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6">
+        <v>2</v>
+      </c>
       <c r="F26" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="6"/>
+      <c r="I26" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J26" s="17"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -1842,18 +2049,22 @@
         <v>152</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
       <c r="F27" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="6"/>
+      <c r="I27" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="J27" s="17"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -1867,18 +2078,22 @@
         <v>162</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6">
+        <v>2</v>
+      </c>
       <c r="F28" s="6" t="s">
         <v>61</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="6"/>
+      <c r="I28" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="J28" s="17"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -1892,16 +2107,20 @@
         <v>154</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
       <c r="F29" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="6"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="J29" s="17"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -1915,16 +2134,20 @@
         <v>163</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="E30" s="6">
+        <v>2</v>
+      </c>
       <c r="F30" s="6" t="s">
         <v>89</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="6"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J30" s="17"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -1938,41 +2161,47 @@
         <v>157</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
       <c r="F31" s="6" t="s">
         <v>93</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="6"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="J31" s="17"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>45961</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="6"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="17"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
October 16th Work. (#88)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7283C2D1-F1C8-4577-9C38-D6FC8021F430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53623F7-A468-481A-9A6B-C2D4CC1A6B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -545,9 +545,6 @@
     <t>Initiation magique, Méta-magie</t>
   </si>
   <si>
-    <t>Talents T2 (2)</t>
-  </si>
-  <si>
     <t>Infatigable, Infirme</t>
   </si>
   <si>
@@ -594,6 +591,9 @@
   </si>
   <si>
     <t>Accélération, Chargement rapide</t>
+  </si>
+  <si>
+    <t>Maladroit</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>106</v>
@@ -1751,24 +1751,24 @@
       <c r="B17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>107</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="8" t="s">
         <v>130</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>165</v>
@@ -1800,8 +1800,8 @@
       <c r="H18" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="18" t="s">
-        <v>181</v>
+      <c r="I18" s="14" t="s">
+        <v>180</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="6"/>
@@ -1830,7 +1830,7 @@
         <v>132</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="6"/>
@@ -1859,7 +1859,7 @@
         <v>133</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="6"/>
@@ -1888,7 +1888,7 @@
         <v>134</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="6"/>
@@ -1917,7 +1917,7 @@
         <v>135</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="6"/>
@@ -1946,7 +1946,7 @@
         <v>136</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="6"/>
@@ -1975,7 +1975,7 @@
         <v>137</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="6"/>
@@ -2004,7 +2004,7 @@
         <v>138</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="6"/>
@@ -2033,7 +2033,7 @@
         <v>139</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="6"/>
@@ -2062,7 +2062,7 @@
         <v>140</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="6"/>
@@ -2091,7 +2091,7 @@
         <v>141</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J28" s="17"/>
       <c r="K28" s="6"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="6"/>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="6"/>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="6"/>
@@ -2201,9 +2201,7 @@
       <c r="M32" s="6"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="I33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
October 17th Work. (#89)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53623F7-A468-481A-9A6B-C2D4CC1A6B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B1FF76-012B-413B-87CA-A4B334445B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Progression" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="188">
   <si>
     <t>Date</t>
   </si>
@@ -554,9 +555,6 @@
     <t>Attaque incapacitante / sanglante</t>
   </si>
   <si>
-    <t>Attaque magie / précise</t>
-  </si>
-  <si>
     <t>Frappe précise, Lancer précis</t>
   </si>
   <si>
@@ -594,6 +592,15 @@
   </si>
   <si>
     <t>Maladroit</t>
+  </si>
+  <si>
+    <t>Duelliste</t>
+  </si>
+  <si>
+    <t>Malchanceux, Malentendant</t>
+  </si>
+  <si>
+    <t>Attaque magique / précise</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84369EDC-CDC8-4C47-A733-5DEB44CD56DA}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1756,7 +1765,7 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>107</v>
@@ -1768,7 +1777,7 @@
         <v>130</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>165</v>
@@ -1784,26 +1793,28 @@
       <c r="B18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6">
-        <v>2</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="8" t="s">
         <v>131</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="J18" s="17"/>
+        <v>179</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -1813,7 +1824,7 @@
         <v>45948</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D19" s="6"/>
@@ -1829,8 +1840,8 @@
       <c r="H19" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>170</v>
+      <c r="I19" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="6"/>
@@ -1842,7 +1853,7 @@
         <v>45949</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>116</v>
       </c>
       <c r="D20" s="6"/>
@@ -1859,7 +1870,7 @@
         <v>133</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="6"/>
@@ -1888,7 +1899,7 @@
         <v>134</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="6"/>
@@ -1917,7 +1928,7 @@
         <v>135</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="6"/>
@@ -1946,7 +1957,7 @@
         <v>136</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="6"/>
@@ -1975,7 +1986,7 @@
         <v>137</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="6"/>
@@ -2004,7 +2015,7 @@
         <v>138</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="6"/>
@@ -2033,7 +2044,7 @@
         <v>139</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="6"/>
@@ -2062,7 +2073,7 @@
         <v>140</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="6"/>
@@ -2091,7 +2102,7 @@
         <v>141</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="J28" s="17"/>
       <c r="K28" s="6"/>
@@ -2145,7 +2156,7 @@
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="6"/>
@@ -2172,7 +2183,7 @@
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="18" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="6"/>

</xml_diff>

<commit_message>
October 18th Work. (#90)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B1FF76-012B-413B-87CA-A4B334445B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AED5B8-7096-42DC-AD14-90F2CB6E31A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Progression" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="198">
   <si>
     <t>Date</t>
   </si>
@@ -601,13 +600,43 @@
   </si>
   <si>
     <t>Attaque magique / précise</t>
+  </si>
+  <si>
+    <t>Élémancien</t>
+  </si>
+  <si>
+    <t>Haruspice</t>
+  </si>
+  <si>
+    <t>Illusionniste</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Magelame</t>
+  </si>
+  <si>
+    <t>Prêtre</t>
+  </si>
+  <si>
+    <t>Soldat</t>
+  </si>
+  <si>
+    <t>Sorcier</t>
+  </si>
+  <si>
+    <t>Troubadour</t>
+  </si>
+  <si>
+    <t>Médecine de brousse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,14 +669,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -804,7 +825,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,19 +845,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1202,9 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84369EDC-CDC8-4C47-A733-5DEB44CD56DA}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1242,7 +1255,7 @@
       <c r="H1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>68</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1281,7 +1294,7 @@
       <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>70</v>
       </c>
       <c r="J2" s="9" t="s">
@@ -1314,7 +1327,7 @@
       <c r="H3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>27</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -1347,7 +1360,7 @@
       <c r="H4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>71</v>
       </c>
       <c r="J4" s="9" t="s">
@@ -1380,7 +1393,7 @@
       <c r="H5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>50</v>
       </c>
       <c r="J5" s="9" t="s">
@@ -1413,7 +1426,7 @@
       <c r="H6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>72</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -1446,10 +1459,10 @@
       <c r="H7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>44</v>
       </c>
       <c r="K7" s="6"/>
@@ -1479,10 +1492,10 @@
       <c r="H8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="K8" s="6"/>
@@ -1512,10 +1525,10 @@
       <c r="H9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="9" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="6"/>
@@ -1545,10 +1558,10 @@
       <c r="H10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="9" t="s">
         <v>80</v>
       </c>
       <c r="K10" s="6"/>
@@ -1578,10 +1591,10 @@
       <c r="H11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="9" t="s">
         <v>92</v>
       </c>
       <c r="K11" s="6"/>
@@ -1611,10 +1624,10 @@
       <c r="H12" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="9" t="s">
         <v>122</v>
       </c>
       <c r="K12" s="6"/>
@@ -1644,10 +1657,10 @@
       <c r="H13" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="9" t="s">
         <v>123</v>
       </c>
       <c r="K13" s="6"/>
@@ -1677,10 +1690,10 @@
       <c r="H14" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="9" t="s">
         <v>124</v>
       </c>
       <c r="K14" s="6"/>
@@ -1710,10 +1723,10 @@
       <c r="H15" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="9" t="s">
         <v>166</v>
       </c>
       <c r="K15" s="6"/>
@@ -1743,10 +1756,10 @@
       <c r="H16" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="9" t="s">
         <v>164</v>
       </c>
       <c r="K16" s="6"/>
@@ -1776,10 +1789,10 @@
       <c r="H17" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="9" t="s">
         <v>165</v>
       </c>
       <c r="K17" s="6"/>
@@ -1809,10 +1822,10 @@
       <c r="H18" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="9" t="s">
         <v>185</v>
       </c>
       <c r="K18" s="6"/>
@@ -1828,22 +1841,24 @@
         <v>115</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="J19" s="17"/>
+      <c r="J19" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1866,13 +1881,15 @@
       <c r="G20" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="I20" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="J20" s="17"/>
+      <c r="I20" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -1895,13 +1912,15 @@
       <c r="G21" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="J21" s="17"/>
+      <c r="I21" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>190</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -1924,13 +1943,15 @@
       <c r="G22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="J22" s="17"/>
+      <c r="I22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -1953,13 +1974,15 @@
       <c r="G23" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="J23" s="17"/>
+      <c r="I23" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>192</v>
+      </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -1982,13 +2005,15 @@
       <c r="G24" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="J24" s="17"/>
+      <c r="I24" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -2011,13 +2036,15 @@
       <c r="G25" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="I25" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="J25" s="17"/>
+      <c r="I25" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>194</v>
+      </c>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -2040,13 +2067,15 @@
       <c r="G26" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="I26" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="J26" s="17"/>
+      <c r="I26" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>195</v>
+      </c>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -2069,13 +2098,15 @@
       <c r="G27" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="I27" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="J27" s="17"/>
+      <c r="I27" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>196</v>
+      </c>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -2098,13 +2129,13 @@
       <c r="G28" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="J28" s="17"/>
+      <c r="I28" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="J28" s="9"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -2127,11 +2158,11 @@
       <c r="G29" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H29" s="16"/>
-      <c r="I29" s="18" t="s">
+      <c r="H29" s="14"/>
+      <c r="I29" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="J29" s="17"/>
+      <c r="J29" s="9"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -2154,11 +2185,11 @@
       <c r="G30" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="18" t="s">
+      <c r="H30" s="14"/>
+      <c r="I30" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="J30" s="17"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -2181,11 +2212,11 @@
       <c r="G31" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H31" s="16"/>
-      <c r="I31" s="18" t="s">
+      <c r="H31" s="14"/>
+      <c r="I31" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="J31" s="17"/>
+      <c r="J31" s="9"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
@@ -2204,9 +2235,9 @@
       <c r="G32" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H32" s="16"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="17"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="9"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>

</xml_diff>

<commit_message>
October 19th Work. (#91)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AED5B8-7096-42DC-AD14-90F2CB6E31A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D459C4-CD84-453E-990A-6A1023DE4C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
   <si>
     <t>Date</t>
   </si>
@@ -630,6 +630,12 @@
   </si>
   <si>
     <t>Médecine de brousse</t>
+  </si>
+  <si>
+    <t>Menace ingénieuse</t>
+  </si>
+  <si>
+    <t>Mots d’encouragement</t>
   </si>
 </sst>
 </file>
@@ -1872,22 +1878,22 @@
         <v>116</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6">
-        <v>2</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="8" t="s">
         <v>133</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="9" t="s">
         <v>189</v>
       </c>
       <c r="K20" s="6"/>
@@ -1903,8 +1909,8 @@
         <v>117</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6">
-        <v>1</v>
+      <c r="E21" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>110</v>
@@ -1915,7 +1921,7 @@
       <c r="H21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="12" t="s">
         <v>187</v>
       </c>
       <c r="J21" s="15" t="s">

</xml_diff>

<commit_message>
October 20th Work. (#92)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D459C4-CD84-453E-990A-6A1023DE4C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D717B435-B543-4FF3-92A0-67636CF134F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -632,10 +632,10 @@
     <t>Médecine de brousse</t>
   </si>
   <si>
-    <t>Menace ingénieuse</t>
-  </si>
-  <si>
     <t>Mots d’encouragement</t>
+  </si>
+  <si>
+    <t>Menace ingénieuse, Muet</t>
   </si>
 </sst>
 </file>
@@ -1878,8 +1878,8 @@
         <v>116</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="5" t="s">
-        <v>198</v>
+      <c r="E20" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>109</v>
@@ -1905,26 +1905,26 @@
         <v>45950</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="F21" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="8" t="s">
         <v>134</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="9" t="s">
         <v>190</v>
       </c>
       <c r="K21" s="6"/>
@@ -1952,7 +1952,7 @@
       <c r="H22" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="12" t="s">
         <v>174</v>
       </c>
       <c r="J22" s="15" t="s">

</xml_diff>

<commit_message>
October 21st Work. (#93)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D717B435-B543-4FF3-92A0-67636CF134F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8369D701-115E-44DA-BE42-C1FA39E07796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="201">
   <si>
     <t>Date</t>
   </si>
@@ -636,6 +636,9 @@
   </si>
   <si>
     <t>Menace ingénieuse, Muet</t>
+  </si>
+  <si>
+    <t>Mysticisme, Orateur</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1284,7 @@
       <c r="A2" s="3">
         <v>45931</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1314,7 +1317,7 @@
       <c r="A3" s="3">
         <v>45932</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1324,7 +1327,7 @@
       <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1347,7 +1350,7 @@
       <c r="A4" s="3">
         <v>45933</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1357,7 +1360,7 @@
       <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1380,7 +1383,7 @@
       <c r="A5" s="3">
         <v>45934</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1390,7 +1393,7 @@
       <c r="E5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1413,7 +1416,7 @@
       <c r="A6" s="3">
         <v>45935</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1423,7 +1426,7 @@
       <c r="E6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1446,7 +1449,7 @@
       <c r="A7" s="3">
         <v>45936</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1456,7 +1459,7 @@
       <c r="E7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1479,7 +1482,7 @@
       <c r="A8" s="3">
         <v>45937</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1489,7 +1492,7 @@
       <c r="E8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1512,7 +1515,7 @@
       <c r="A9" s="3">
         <v>45938</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1522,7 +1525,7 @@
       <c r="E9" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1545,7 +1548,7 @@
       <c r="A10" s="3">
         <v>45939</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1555,7 +1558,7 @@
       <c r="E10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>84</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -1578,7 +1581,7 @@
       <c r="A11" s="3">
         <v>45940</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1588,7 +1591,7 @@
       <c r="E11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1611,7 +1614,7 @@
       <c r="A12" s="3">
         <v>45941</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>94</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1621,7 +1624,7 @@
       <c r="E12" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>93</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -1644,7 +1647,7 @@
       <c r="A13" s="3">
         <v>45942</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1677,7 +1680,7 @@
       <c r="A14" s="3">
         <v>45943</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1710,7 +1713,7 @@
       <c r="A15" s="3">
         <v>45944</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1743,7 +1746,7 @@
       <c r="A16" s="3">
         <v>45945</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1776,7 +1779,7 @@
       <c r="A17" s="3">
         <v>45946</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1809,7 +1812,7 @@
       <c r="A18" s="3">
         <v>45947</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1842,7 +1845,7 @@
       <c r="A19" s="3">
         <v>45948</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
         <v>115</v>
       </c>
@@ -1873,7 +1876,7 @@
       <c r="A20" s="3">
         <v>45949</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
         <v>116</v>
       </c>
@@ -1904,7 +1907,7 @@
       <c r="A21" s="3">
         <v>45950</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>117</v>
       </c>
@@ -1935,27 +1938,27 @@
       <c r="A22" s="3">
         <v>45951</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>148</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="6">
-        <v>2</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="E22" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="8" t="s">
         <v>135</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="9" t="s">
         <v>191</v>
       </c>
       <c r="K22" s="6"/>
@@ -1966,7 +1969,7 @@
       <c r="A23" s="3">
         <v>45952</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
         <v>160</v>
       </c>
@@ -1983,7 +1986,7 @@
       <c r="H23" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="12" t="s">
         <v>181</v>
       </c>
       <c r="J23" s="15" t="s">
@@ -1997,7 +2000,7 @@
       <c r="A24" s="3">
         <v>45953</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
         <v>150</v>
       </c>
@@ -2028,7 +2031,7 @@
       <c r="A25" s="3">
         <v>45954</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
         <v>161</v>
       </c>
@@ -2059,7 +2062,7 @@
       <c r="A26" s="3">
         <v>45955</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
         <v>151</v>
       </c>
@@ -2090,7 +2093,7 @@
       <c r="A27" s="3">
         <v>45956</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
         <v>152</v>
       </c>
@@ -2121,7 +2124,7 @@
       <c r="A28" s="3">
         <v>45957</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>162</v>
       </c>
@@ -2150,7 +2153,7 @@
       <c r="A29" s="3">
         <v>45958</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
         <v>154</v>
       </c>
@@ -2177,7 +2180,7 @@
       <c r="A30" s="3">
         <v>45959</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="5" t="s">
         <v>163</v>
       </c>
@@ -2204,7 +2207,7 @@
       <c r="A31" s="3">
         <v>45960</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
         <v>157</v>
       </c>
@@ -2231,7 +2234,7 @@
       <c r="A32" s="3">
         <v>45961</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6">

</xml_diff>

<commit_message>
October 22th Work. (#96)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8369D701-115E-44DA-BE42-C1FA39E07796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17960DA4-941C-4012-94D0-117B0405A7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="203">
   <si>
     <t>Date</t>
   </si>
@@ -639,6 +639,12 @@
   </si>
   <si>
     <t>Mysticisme, Orateur</t>
+  </si>
+  <si>
+    <t>Pauvreté, Richesse</t>
+  </si>
+  <si>
+    <t>Pensée claire</t>
   </si>
 </sst>
 </file>
@@ -1970,26 +1976,26 @@
         <v>45952</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>160</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E23" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="9" t="s">
         <v>192</v>
       </c>
       <c r="K23" s="6"/>
@@ -2001,26 +2007,26 @@
         <v>45953</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6">
-        <v>2</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="8" t="s">
         <v>137</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="J24" s="9" t="s">
         <v>193</v>
       </c>
       <c r="K24" s="6"/>
@@ -2048,7 +2054,7 @@
       <c r="H25" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="I25" s="12" t="s">
         <v>173</v>
       </c>
       <c r="J25" s="15" t="s">

</xml_diff>

<commit_message>
October 23rd Work. (#97)
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\SkillCraftRPG\SkillCraftRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17960DA4-941C-4012-94D0-117B0405A7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EDFC32-E677-4EDA-AB19-7F5798C0C8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{D8D7B8D7-BAEA-4549-B48E-785F40F0C8C6}"/>
   </bookViews>
@@ -1992,7 +1992,7 @@
       <c r="H23" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="12" t="s">
         <v>181</v>
       </c>
       <c r="J23" s="9" t="s">
@@ -2023,7 +2023,7 @@
       <c r="H24" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="12" t="s">
         <v>180</v>
       </c>
       <c r="J24" s="9" t="s">

</xml_diff>